<commit_message>
Atualizar análise de agrupamento hierárquico para os meses de maio, junho e julho de 2025
- Modificado o script para incluir filtro de volume mínimo no cálculo do benchmark, removendo rotas com baixo volume.
- Adicionadas novas funções para configurar volumes mínimos e benchmark inteligente.
- Implementada análise da distribuição dos volumes para otimização do benchmark.
- Criada nova planilha com fórmulas e uma versão limpa com apenas as colunas essenciais.
- Documentação atualizada para refletir as novas funcionalidades e melhorias no sistema de benchmark inteligente.
</commit_message>
<xml_diff>
--- a/outputs/dashboard_hierarquico.xlsx
+++ b/outputs/dashboard_hierarquico.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amaro/Documents/Acelomittal - Sistemas/Projetos/arcelor-frete/outputs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74CF18D-74BB-1E4C-91C0-CF10D8E53771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="620" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -628,8 +634,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -692,13 +698,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -736,7 +750,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -770,6 +784,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -804,9 +819,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -979,14 +995,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1012,7 +1035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1023,22 +1046,22 @@
         <v>80</v>
       </c>
       <c r="D2">
-        <v>212.451</v>
+        <v>212.45099999999999</v>
       </c>
       <c r="E2">
         <v>212.8602830770389</v>
       </c>
       <c r="F2">
-        <v>0.2035273336645188</v>
+        <v>0.20352733366451881</v>
       </c>
       <c r="G2">
-        <v>-0.4272896510079818</v>
+        <v>-0.42728965100798177</v>
       </c>
       <c r="H2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1049,7 +1072,7 @@
         <v>81</v>
       </c>
       <c r="D3">
-        <v>61.345</v>
+        <v>61.344999999999999</v>
       </c>
       <c r="E3">
         <v>112.6067324150297</v>
@@ -1058,13 +1081,13 @@
         <v>0.1039727327174408</v>
       </c>
       <c r="G3">
-        <v>-0.5268442519550598</v>
+        <v>-0.52684425195505979</v>
       </c>
       <c r="H3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1075,13 +1098,13 @@
         <v>82</v>
       </c>
       <c r="D4">
-        <v>210.943</v>
+        <v>210.94300000000001</v>
       </c>
       <c r="E4">
-        <v>469.1524250626945</v>
+        <v>469.15242506269448</v>
       </c>
       <c r="F4">
-        <v>0.4967751081778135</v>
+        <v>0.49677510817781351</v>
       </c>
       <c r="G4">
         <v>-0.1340418764946871</v>
@@ -1090,7 +1113,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1101,22 +1124,22 @@
         <v>83</v>
       </c>
       <c r="D5">
-        <v>632.337</v>
+        <v>632.33699999999999</v>
       </c>
       <c r="E5">
-        <v>373.0078581515868</v>
+        <v>373.00785815158679</v>
       </c>
       <c r="F5">
-        <v>0.3343883450201722</v>
+        <v>0.33438834502017217</v>
       </c>
       <c r="G5">
-        <v>-0.2964286396523284</v>
+        <v>-0.29642863965232841</v>
       </c>
       <c r="H5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1127,22 +1150,22 @@
         <v>84</v>
       </c>
       <c r="D6">
-        <v>2.152</v>
+        <v>2.1520000000000001</v>
       </c>
       <c r="E6">
         <v>109.5817843866171</v>
       </c>
       <c r="F6">
-        <v>0.1152620115792543</v>
+        <v>0.11526201157925429</v>
       </c>
       <c r="G6">
-        <v>-0.5155549730932463</v>
+        <v>-0.51555497309324627</v>
       </c>
       <c r="H6" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1156,19 +1179,19 @@
         <v>3301.353999999998</v>
       </c>
       <c r="E7">
-        <v>256.0071291960815</v>
+        <v>256.00712919608151</v>
       </c>
       <c r="F7">
-        <v>0.3100632453223331</v>
+        <v>0.31006324532233309</v>
       </c>
       <c r="G7">
-        <v>-0.3207537393501675</v>
+        <v>-0.32075373935016749</v>
       </c>
       <c r="H7" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1179,13 +1202,13 @@
         <v>86</v>
       </c>
       <c r="D8">
-        <v>51.482</v>
+        <v>51.481999999999999</v>
       </c>
       <c r="E8">
-        <v>426.5605454333553</v>
+        <v>426.56054543335529</v>
       </c>
       <c r="F8">
-        <v>0.5115616250519948</v>
+        <v>0.51156162505199476</v>
       </c>
       <c r="G8">
         <v>-0.1192553596205058</v>
@@ -1194,7 +1217,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1205,22 +1228,22 @@
         <v>87</v>
       </c>
       <c r="D9">
-        <v>8890.307999999997</v>
+        <v>8890.3079999999973</v>
       </c>
       <c r="E9">
-        <v>321.2063406577143</v>
+        <v>321.20634065771429</v>
       </c>
       <c r="F9">
-        <v>0.5364758651717053</v>
+        <v>0.53647586517170531</v>
       </c>
       <c r="G9">
-        <v>-0.09434111950079527</v>
+        <v>-9.4341119500795267E-2</v>
       </c>
       <c r="H9" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1234,19 +1257,19 @@
         <v>389.9969999999999</v>
       </c>
       <c r="E10">
-        <v>70.94739190301466</v>
+        <v>70.947391903014662</v>
       </c>
       <c r="F10">
-        <v>0.6218546051627192</v>
+        <v>0.62185460516271918</v>
       </c>
       <c r="G10">
-        <v>-0.008962379509781404</v>
+        <v>-8.9623795097814041E-3</v>
       </c>
       <c r="H10" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1260,10 +1283,10 @@
         <v>24.363</v>
       </c>
       <c r="E11">
-        <v>59.07605795673768</v>
+        <v>59.076057956737678</v>
       </c>
       <c r="F11">
-        <v>0.4112327919247207</v>
+        <v>0.41123279192472068</v>
       </c>
       <c r="G11">
         <v>-0.2195841927477799</v>
@@ -1272,7 +1295,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1283,7 +1306,7 @@
         <v>90</v>
       </c>
       <c r="D12">
-        <v>45690.91900000012</v>
+        <v>45690.919000000118</v>
       </c>
       <c r="E12">
         <v>121.0144674481156</v>
@@ -1298,7 +1321,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1309,22 +1332,22 @@
         <v>91</v>
       </c>
       <c r="D13">
-        <v>289078.6170000001</v>
+        <v>289078.61700000009</v>
       </c>
       <c r="E13">
-        <v>97.67654063461931</v>
+        <v>97.676540634619315</v>
       </c>
       <c r="F13">
-        <v>0.7501347082803281</v>
+        <v>0.75013470828032813</v>
       </c>
       <c r="G13">
-        <v>0.1193177236078276</v>
+        <v>0.11931772360782759</v>
       </c>
       <c r="H13" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1335,22 +1358,22 @@
         <v>92</v>
       </c>
       <c r="D14">
-        <v>169.944</v>
+        <v>169.94399999999999</v>
       </c>
       <c r="E14">
-        <v>85.84174786988659</v>
+        <v>85.841747869886589</v>
       </c>
       <c r="F14">
-        <v>0.6052567414518153</v>
+        <v>0.60525674145181529</v>
       </c>
       <c r="G14">
-        <v>-0.02556024322068529</v>
+        <v>-2.5560243220685289E-2</v>
       </c>
       <c r="H14" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1361,22 +1384,22 @@
         <v>93</v>
       </c>
       <c r="D15">
-        <v>88.298</v>
+        <v>88.298000000000002</v>
       </c>
       <c r="E15">
-        <v>97.64400099662507</v>
+        <v>97.644000996625067</v>
       </c>
       <c r="F15">
-        <v>0.6856829934315404</v>
+        <v>0.68568299343154038</v>
       </c>
       <c r="G15">
-        <v>0.0548660087590398</v>
+        <v>5.4866008759039797E-2</v>
       </c>
       <c r="H15" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1387,22 +1410,22 @@
         <v>94</v>
       </c>
       <c r="D16">
-        <v>166960.2820000001</v>
+        <v>166960.28200000009</v>
       </c>
       <c r="E16">
-        <v>122.3359228034846</v>
+        <v>122.33592280348461</v>
       </c>
       <c r="F16">
         <v>1.050030665998555</v>
       </c>
       <c r="G16">
-        <v>0.4192136813260549</v>
+        <v>0.41921368132605491</v>
       </c>
       <c r="H16" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1413,22 +1436,22 @@
         <v>95</v>
       </c>
       <c r="D17">
-        <v>28470.91000000001</v>
+        <v>28470.910000000011</v>
       </c>
       <c r="E17">
         <v>111.2308949731499</v>
       </c>
       <c r="F17">
-        <v>0.9382297937914278</v>
+        <v>0.93822979379142779</v>
       </c>
       <c r="G17">
-        <v>0.3074128091189272</v>
+        <v>0.30741280911892721</v>
       </c>
       <c r="H17" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1439,22 +1462,22 @@
         <v>96</v>
       </c>
       <c r="D18">
-        <v>392.0740000000001</v>
+        <v>392.07400000000013</v>
       </c>
       <c r="E18">
-        <v>98.17386513770357</v>
+        <v>98.173865137703572</v>
       </c>
       <c r="F18">
-        <v>0.6180871038354497</v>
+        <v>0.61808710383544974</v>
       </c>
       <c r="G18">
-        <v>-0.01272988083705084</v>
+        <v>-1.2729880837050841E-2</v>
       </c>
       <c r="H18" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1468,19 +1491,19 @@
         <v>8390.695000000007</v>
       </c>
       <c r="E19">
-        <v>162.5162981135651</v>
+        <v>162.51629811356511</v>
       </c>
       <c r="F19">
         <v>1.228559426933111</v>
       </c>
       <c r="G19">
-        <v>0.5977424422606102</v>
+        <v>0.59774244226061024</v>
       </c>
       <c r="H19" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1497,16 +1520,16 @@
         <v>113.7459131247081</v>
       </c>
       <c r="F20">
-        <v>0.08826263646259205</v>
+        <v>8.8262636462592053E-2</v>
       </c>
       <c r="G20">
-        <v>-0.5425543482099086</v>
+        <v>-0.54255434820990855</v>
       </c>
       <c r="H20" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1520,19 +1543,19 @@
         <v>3828.913</v>
       </c>
       <c r="E21">
-        <v>416.6402710116421</v>
+        <v>416.64027101164208</v>
       </c>
       <c r="F21">
-        <v>0.3155184885441693</v>
+        <v>0.31551848854416931</v>
       </c>
       <c r="G21">
-        <v>-0.3152984961283313</v>
+        <v>-0.31529849612833127</v>
       </c>
       <c r="H21" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1543,13 +1566,13 @@
         <v>100</v>
       </c>
       <c r="D22">
-        <v>2656.155</v>
+        <v>2656.1550000000002</v>
       </c>
       <c r="E22">
-        <v>579.1650073132029</v>
+        <v>579.16500731320286</v>
       </c>
       <c r="F22">
-        <v>0.4357169619493521</v>
+        <v>0.43571696194935211</v>
       </c>
       <c r="G22">
         <v>-0.1951000227231485</v>
@@ -1558,7 +1581,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1572,19 +1595,19 @@
         <v>5883.954999999999</v>
       </c>
       <c r="E23">
-        <v>359.6513926432133</v>
+        <v>359.65139264321328</v>
       </c>
       <c r="F23">
-        <v>0.2766121489240611</v>
+        <v>0.27661214892406111</v>
       </c>
       <c r="G23">
-        <v>-0.3542048357484395</v>
+        <v>-0.35420483574843947</v>
       </c>
       <c r="H23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1595,22 +1618,22 @@
         <v>102</v>
       </c>
       <c r="D24">
-        <v>790.4820000000001</v>
+        <v>790.48200000000008</v>
       </c>
       <c r="E24">
-        <v>304.9815935087707</v>
+        <v>304.98159350877069</v>
       </c>
       <c r="F24">
-        <v>0.2358838897889917</v>
+        <v>0.23588388978899169</v>
       </c>
       <c r="G24">
-        <v>-0.3949330948835088</v>
+        <v>-0.39493309488350881</v>
       </c>
       <c r="H24" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1621,22 +1644,22 @@
         <v>103</v>
       </c>
       <c r="D25">
-        <v>20.583</v>
+        <v>20.582999999999998</v>
       </c>
       <c r="E25">
         <v>226.4125734829714</v>
       </c>
       <c r="F25">
-        <v>0.3566597042330059</v>
+        <v>0.35665970423300591</v>
       </c>
       <c r="G25">
-        <v>-0.2741572804394947</v>
+        <v>-0.27415728043949472</v>
       </c>
       <c r="H25" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1647,22 +1670,22 @@
         <v>104</v>
       </c>
       <c r="D26">
-        <v>455.3199999999999</v>
+        <v>455.31999999999988</v>
       </c>
       <c r="E26">
         <v>252.3544540103664</v>
       </c>
       <c r="F26">
-        <v>0.3778468336295959</v>
+        <v>0.37784683362959592</v>
       </c>
       <c r="G26">
-        <v>-0.2529701510429047</v>
+        <v>-0.25297015104290471</v>
       </c>
       <c r="H26" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1673,13 +1696,13 @@
         <v>105</v>
       </c>
       <c r="D27">
-        <v>6221.529000000004</v>
+        <v>6221.5290000000041</v>
       </c>
       <c r="E27">
-        <v>274.0137352088207</v>
+        <v>274.01373520882072</v>
       </c>
       <c r="F27">
-        <v>0.3264419435531777</v>
+        <v>0.32644194355317768</v>
       </c>
       <c r="G27">
         <v>-0.3043750411193229</v>
@@ -1688,7 +1711,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1702,19 +1725,19 @@
         <v>11.077</v>
       </c>
       <c r="E28">
-        <v>818.7613974902952</v>
+        <v>818.76139749029517</v>
       </c>
       <c r="F28">
         <v>0.4071053867386652</v>
       </c>
       <c r="G28">
-        <v>-0.2237115979338354</v>
+        <v>-0.22371159793383541</v>
       </c>
       <c r="H28" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1725,22 +1748,22 @@
         <v>107</v>
       </c>
       <c r="D29">
-        <v>4.086</v>
+        <v>4.0860000000000003</v>
       </c>
       <c r="E29">
         <v>109.5790504160548</v>
       </c>
       <c r="F29">
-        <v>0.3157588317457506</v>
+        <v>0.31575883174575059</v>
       </c>
       <c r="G29">
-        <v>-0.3150581529267499</v>
+        <v>-0.31505815292674988</v>
       </c>
       <c r="H29" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1751,22 +1774,22 @@
         <v>108</v>
       </c>
       <c r="D30">
-        <v>1107.987</v>
+        <v>1107.9870000000001</v>
       </c>
       <c r="E30">
-        <v>109.7947268334376</v>
+        <v>109.79472683343759</v>
       </c>
       <c r="F30">
-        <v>0.04909409744056237</v>
+        <v>4.9094097440562368E-2</v>
       </c>
       <c r="G30">
-        <v>-0.5817228872319382</v>
+        <v>-0.58172288723193821</v>
       </c>
       <c r="H30" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1780,19 +1803,19 @@
         <v>7886.896999999999</v>
       </c>
       <c r="E31">
-        <v>262.5374427991136</v>
+        <v>262.53744279911359</v>
       </c>
       <c r="F31">
-        <v>0.3792567379602981</v>
+        <v>0.37925673796029807</v>
       </c>
       <c r="G31">
-        <v>-0.2515602467122025</v>
+        <v>-0.25156024671220251</v>
       </c>
       <c r="H31" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1803,22 +1826,22 @@
         <v>110</v>
       </c>
       <c r="D32">
-        <v>3978.511000000002</v>
+        <v>3978.5110000000018</v>
       </c>
       <c r="E32">
-        <v>323.3452540410216</v>
+        <v>323.34525404102158</v>
       </c>
       <c r="F32">
-        <v>0.4487148319407784</v>
+        <v>0.44871483194077838</v>
       </c>
       <c r="G32">
-        <v>-0.1821021527317221</v>
+        <v>-0.18210215273172209</v>
       </c>
       <c r="H32" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1829,22 +1852,22 @@
         <v>111</v>
       </c>
       <c r="D33">
-        <v>13526.35800000001</v>
+        <v>13526.358000000009</v>
       </c>
       <c r="E33">
         <v>228.5709619692152</v>
       </c>
       <c r="F33">
-        <v>0.3334986379230148</v>
+        <v>0.33349863792301482</v>
       </c>
       <c r="G33">
-        <v>-0.2973183467494858</v>
+        <v>-0.29731834674948582</v>
       </c>
       <c r="H33" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1858,19 +1881,19 @@
         <v>101.372</v>
       </c>
       <c r="E34">
-        <v>466.3880558734166</v>
+        <v>466.38805587341659</v>
       </c>
       <c r="F34">
-        <v>0.3230104848629399</v>
+        <v>0.32301048486293987</v>
       </c>
       <c r="G34">
-        <v>-0.3078064998095607</v>
+        <v>-0.30780649980956071</v>
       </c>
       <c r="H34" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1881,22 +1904,22 @@
         <v>113</v>
       </c>
       <c r="D35">
-        <v>2.247</v>
+        <v>2.2469999999999999</v>
       </c>
       <c r="E35">
         <v>109.5816644414775</v>
       </c>
       <c r="F35">
-        <v>0.06543216304499005</v>
+        <v>6.5432163044990055E-2</v>
       </c>
       <c r="G35">
-        <v>-0.5653848216275106</v>
+        <v>-0.56538482162751058</v>
       </c>
       <c r="H35" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1907,22 +1930,22 @@
         <v>114</v>
       </c>
       <c r="D36">
-        <v>180.579</v>
+        <v>180.57900000000001</v>
       </c>
       <c r="E36">
-        <v>286.7162294618976</v>
+        <v>286.71622946189763</v>
       </c>
       <c r="F36">
-        <v>0.1847299593268514</v>
+        <v>0.18472995932685141</v>
       </c>
       <c r="G36">
-        <v>-0.4460870253456491</v>
+        <v>-0.44608702534564909</v>
       </c>
       <c r="H36" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1936,19 +1959,19 @@
         <v>1402.211</v>
       </c>
       <c r="E37">
-        <v>365.0100020610308</v>
+        <v>365.01000206103078</v>
       </c>
       <c r="F37">
-        <v>0.2322552332739654</v>
+        <v>0.23225523327396541</v>
       </c>
       <c r="G37">
-        <v>-0.3985617513985352</v>
+        <v>-0.39856175139853522</v>
       </c>
       <c r="H37" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -1959,22 +1982,22 @@
         <v>116</v>
       </c>
       <c r="D38">
-        <v>324.443</v>
+        <v>324.44299999999998</v>
       </c>
       <c r="E38">
-        <v>562.0536735266288</v>
+        <v>562.05367352662881</v>
       </c>
       <c r="F38">
         <v>0.3588560821425037</v>
       </c>
       <c r="G38">
-        <v>-0.2719609025299969</v>
+        <v>-0.27196090252999688</v>
       </c>
       <c r="H38" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1991,16 +2014,16 @@
         <v>479.8613995676684</v>
       </c>
       <c r="F39">
-        <v>0.2838571712488345</v>
+        <v>0.28385717124883447</v>
       </c>
       <c r="G39">
-        <v>-0.3469598134236661</v>
+        <v>-0.34695981342366611</v>
       </c>
       <c r="H39" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2011,22 +2034,22 @@
         <v>118</v>
       </c>
       <c r="D40">
-        <v>479.0300000000001</v>
+        <v>479.03000000000009</v>
       </c>
       <c r="E40">
-        <v>368.5902553076007</v>
+        <v>368.59025530760073</v>
       </c>
       <c r="F40">
         <v>0.3373150760833083</v>
       </c>
       <c r="G40">
-        <v>-0.2935019085891923</v>
+        <v>-0.29350190858919228</v>
       </c>
       <c r="H40" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -2037,22 +2060,22 @@
         <v>119</v>
       </c>
       <c r="D41">
-        <v>31.336</v>
+        <v>31.335999999999999</v>
       </c>
       <c r="E41">
-        <v>362.2600204237938</v>
+        <v>362.26002042379378</v>
       </c>
       <c r="F41">
-        <v>0.3314291547338337</v>
+        <v>0.33142915473383372</v>
       </c>
       <c r="G41">
-        <v>-0.2993878299386669</v>
+        <v>-0.29938782993866692</v>
       </c>
       <c r="H41" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2063,22 +2086,22 @@
         <v>120</v>
       </c>
       <c r="D42">
-        <v>444.0409999999999</v>
+        <v>444.04099999999988</v>
       </c>
       <c r="E42">
-        <v>295.000506709966</v>
+        <v>295.00050670996598</v>
       </c>
       <c r="F42">
-        <v>0.2685912700794084</v>
+        <v>0.26859127007940842</v>
       </c>
       <c r="G42">
-        <v>-0.3622257145930922</v>
+        <v>-0.36222571459309222</v>
       </c>
       <c r="H42" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2089,13 +2112,13 @@
         <v>121</v>
       </c>
       <c r="D43">
-        <v>2762.028999999999</v>
+        <v>2762.0289999999991</v>
       </c>
       <c r="E43">
         <v>109.7499881427748</v>
       </c>
       <c r="F43">
-        <v>0.4749293043000037</v>
+        <v>0.47492930430000369</v>
       </c>
       <c r="G43">
         <v>-0.1558876803724969</v>
@@ -2104,7 +2127,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -2121,7 +2144,7 @@
         <v>152.0415410205735</v>
       </c>
       <c r="F44">
-        <v>0.7854237340856151</v>
+        <v>0.78542373408561506</v>
       </c>
       <c r="G44">
         <v>0.1546067494131145</v>
@@ -2130,7 +2153,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2141,22 +2164,22 @@
         <v>123</v>
       </c>
       <c r="D45">
-        <v>9871.585999999985</v>
+        <v>9871.5859999999848</v>
       </c>
       <c r="E45">
-        <v>334.9383209547083</v>
+        <v>334.93832095470827</v>
       </c>
       <c r="F45">
-        <v>0.2974897200192482</v>
+        <v>0.29748972001924823</v>
       </c>
       <c r="G45">
-        <v>-0.3333272646532524</v>
+        <v>-0.33332726465325241</v>
       </c>
       <c r="H45" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -2167,22 +2190,22 @@
         <v>124</v>
       </c>
       <c r="D46">
-        <v>69.547</v>
+        <v>69.546999999999997</v>
       </c>
       <c r="E46">
-        <v>611.3997728155061</v>
+        <v>611.39977281550614</v>
       </c>
       <c r="F46">
-        <v>0.6486256989284052</v>
+        <v>0.64862569892840516</v>
       </c>
       <c r="G46">
-        <v>0.01780871425590458</v>
+        <v>1.7808714255904579E-2</v>
       </c>
       <c r="H46" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2193,13 +2216,13 @@
         <v>125</v>
       </c>
       <c r="D47">
-        <v>3.916</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="E47">
-        <v>209.4407558733401</v>
+        <v>209.44075587334009</v>
       </c>
       <c r="F47">
-        <v>0.1538576717896102</v>
+        <v>0.15385767178961021</v>
       </c>
       <c r="G47">
         <v>-0.4769593128828904</v>
@@ -2208,7 +2231,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2219,22 +2242,22 @@
         <v>126</v>
       </c>
       <c r="D48">
-        <v>170.325</v>
+        <v>170.32499999999999</v>
       </c>
       <c r="E48">
-        <v>239.9241450168794</v>
+        <v>239.92414501687941</v>
       </c>
       <c r="F48">
-        <v>0.35130043489645</v>
+        <v>0.35130043489645002</v>
       </c>
       <c r="G48">
-        <v>-0.2795165497760506</v>
+        <v>-0.27951654977605062</v>
       </c>
       <c r="H48" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -2245,22 +2268,22 @@
         <v>127</v>
       </c>
       <c r="D49">
-        <v>99.62100000000001</v>
+        <v>99.621000000000009</v>
       </c>
       <c r="E49">
-        <v>409.3840656086568</v>
+        <v>409.38406560865678</v>
       </c>
       <c r="F49">
-        <v>0.4150755819888884</v>
+        <v>0.41507558198888839</v>
       </c>
       <c r="G49">
-        <v>-0.2157414026836122</v>
+        <v>-0.21574140268361219</v>
       </c>
       <c r="H49" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2274,19 +2297,19 @@
         <v>122.474</v>
       </c>
       <c r="E50">
-        <v>141.8410438133808</v>
+        <v>141.84104381338079</v>
       </c>
       <c r="F50">
-        <v>0.1484326405132952</v>
+        <v>0.14843264051329519</v>
       </c>
       <c r="G50">
-        <v>-0.4823843441592054</v>
+        <v>-0.48238434415920539</v>
       </c>
       <c r="H50" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -2300,10 +2323,10 @@
         <v>43565.58</v>
       </c>
       <c r="E51">
-        <v>152.9081150761679</v>
+        <v>152.90811507616789</v>
       </c>
       <c r="F51">
-        <v>0.7512509461435584</v>
+        <v>0.75125094614355836</v>
       </c>
       <c r="G51">
         <v>0.1204339614710578</v>
@@ -2312,7 +2335,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2323,22 +2346,22 @@
         <v>130</v>
       </c>
       <c r="D52">
-        <v>516.539</v>
+        <v>516.53899999999999</v>
       </c>
       <c r="E52">
-        <v>650.8528107267796</v>
+        <v>650.85281072677958</v>
       </c>
       <c r="F52">
-        <v>0.1899201135946378</v>
+        <v>0.18992011359463781</v>
       </c>
       <c r="G52">
-        <v>-0.4408968710778627</v>
+        <v>-0.44089687107786268</v>
       </c>
       <c r="H52" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2349,22 +2372,22 @@
         <v>131</v>
       </c>
       <c r="D53">
-        <v>27.365</v>
+        <v>27.364999999999998</v>
       </c>
       <c r="E53">
-        <v>210.4699433583044</v>
+        <v>210.46994335830439</v>
       </c>
       <c r="F53">
-        <v>0.2949708257535856</v>
+        <v>0.29497082575358557</v>
       </c>
       <c r="G53">
-        <v>-0.335846158918915</v>
+        <v>-0.33584615891891501</v>
       </c>
       <c r="H53" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2378,19 +2401,19 @@
         <v>3452.092000000001</v>
       </c>
       <c r="E54">
-        <v>253.6695400933694</v>
+        <v>253.66954009336939</v>
       </c>
       <c r="F54">
-        <v>0.3703037382153053</v>
+        <v>0.37030373821530532</v>
       </c>
       <c r="G54">
-        <v>-0.2605132464571953</v>
+        <v>-0.26051324645719531</v>
       </c>
       <c r="H54" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2401,22 +2424,22 @@
         <v>133</v>
       </c>
       <c r="D55">
-        <v>206.258</v>
+        <v>206.25800000000001</v>
       </c>
       <c r="E55">
-        <v>181.3177670684289</v>
+        <v>181.31776706842891</v>
       </c>
       <c r="F55">
         <v>0.1225246711777831</v>
       </c>
       <c r="G55">
-        <v>-0.5082923134947175</v>
+        <v>-0.50829231349471748</v>
       </c>
       <c r="H55" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -2427,22 +2450,22 @@
         <v>134</v>
       </c>
       <c r="D56">
-        <v>36.017</v>
+        <v>36.017000000000003</v>
       </c>
       <c r="E56">
-        <v>351.6311741677541</v>
+        <v>351.63117416775412</v>
       </c>
       <c r="F56">
-        <v>0.6462252181326814</v>
+        <v>0.64622521813268141</v>
       </c>
       <c r="G56">
-        <v>0.01540823346018083</v>
+        <v>1.540823346018083E-2</v>
       </c>
       <c r="H56" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -2453,22 +2476,22 @@
         <v>135</v>
       </c>
       <c r="D57">
-        <v>3719.617</v>
+        <v>3719.6170000000002</v>
       </c>
       <c r="E57">
         <v>261.9969260275991</v>
       </c>
       <c r="F57">
-        <v>0.3633799251423011</v>
+        <v>0.36337992514230111</v>
       </c>
       <c r="G57">
-        <v>-0.2674370595301995</v>
+        <v>-0.26743705953019947</v>
       </c>
       <c r="H57" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -2479,13 +2502,13 @@
         <v>136</v>
       </c>
       <c r="D58">
-        <v>4.454</v>
+        <v>4.4539999999999997</v>
       </c>
       <c r="E58">
-        <v>393.3879658733723</v>
+        <v>393.38796587337231</v>
       </c>
       <c r="F58">
-        <v>0.5307103234995201</v>
+        <v>0.53071032349952008</v>
       </c>
       <c r="G58">
         <v>-0.1001066611729805</v>
@@ -2494,7 +2517,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -2508,19 +2531,19 @@
         <v>43.94</v>
       </c>
       <c r="E59">
-        <v>979.984069185253</v>
+        <v>979.98406918525302</v>
       </c>
       <c r="F59">
-        <v>0.9949440478893167</v>
+        <v>0.99494404788931667</v>
       </c>
       <c r="G59">
-        <v>0.3641270632168161</v>
+        <v>0.36412706321681609</v>
       </c>
       <c r="H59" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -2531,22 +2554,22 @@
         <v>138</v>
       </c>
       <c r="D60">
-        <v>682.0549999999999</v>
+        <v>682.05499999999995</v>
       </c>
       <c r="E60">
         <v>506.8578047224932</v>
       </c>
       <c r="F60">
-        <v>0.1858318987714764</v>
+        <v>0.18583189877147641</v>
       </c>
       <c r="G60">
-        <v>-0.4449850859010241</v>
+        <v>-0.44498508590102409</v>
       </c>
       <c r="H60" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -2557,22 +2580,22 @@
         <v>139</v>
       </c>
       <c r="D61">
-        <v>956.7029999999993</v>
+        <v>956.70299999999929</v>
       </c>
       <c r="E61">
-        <v>582.8751869702513</v>
+        <v>582.87518697025132</v>
       </c>
       <c r="F61">
-        <v>0.4022258874811613</v>
+        <v>0.40222588748116128</v>
       </c>
       <c r="G61">
-        <v>-0.2285910971913392</v>
+        <v>-0.22859109719133919</v>
       </c>
       <c r="H61" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -2583,22 +2606,22 @@
         <v>140</v>
       </c>
       <c r="D62">
-        <v>12813.718</v>
+        <v>12813.718000000001</v>
       </c>
       <c r="E62">
-        <v>374.072487782235</v>
+        <v>374.07248778223499</v>
       </c>
       <c r="F62">
         <v>0.3053251676981461</v>
       </c>
       <c r="G62">
-        <v>-0.3254918169743545</v>
+        <v>-0.32549181697435448</v>
       </c>
       <c r="H62" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -2609,22 +2632,22 @@
         <v>141</v>
       </c>
       <c r="D63">
-        <v>96.28300000000002</v>
+        <v>96.283000000000015</v>
       </c>
       <c r="E63">
-        <v>330.8999511855675</v>
+        <v>330.89995118556749</v>
       </c>
       <c r="F63">
-        <v>0.2820738192882323</v>
+        <v>0.28207381928823227</v>
       </c>
       <c r="G63">
-        <v>-0.3487431653842682</v>
+        <v>-0.34874316538426819</v>
       </c>
       <c r="H63" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -2635,22 +2658,22 @@
         <v>142</v>
       </c>
       <c r="D64">
-        <v>2.251</v>
+        <v>2.2509999999999999</v>
       </c>
       <c r="E64">
-        <v>604.8511772545536</v>
+        <v>604.85117725455359</v>
       </c>
       <c r="F64">
-        <v>0.4820514601022627</v>
+        <v>0.48205146010226269</v>
       </c>
       <c r="G64">
-        <v>-0.1487655245702378</v>
+        <v>-0.14876552457023781</v>
       </c>
       <c r="H64" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -2661,13 +2684,13 @@
         <v>143</v>
       </c>
       <c r="D65">
-        <v>26652.943</v>
+        <v>26652.942999999999</v>
       </c>
       <c r="E65">
-        <v>163.2838336089189</v>
+        <v>163.28383360891891</v>
       </c>
       <c r="F65">
-        <v>0.5016400418092747</v>
+        <v>0.50164004180927468</v>
       </c>
       <c r="G65">
         <v>-0.1291769428632259</v>
@@ -2676,7 +2699,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -2690,19 +2713,19 @@
         <v>2464.252</v>
       </c>
       <c r="E66">
-        <v>257.4626377497106</v>
+        <v>257.46263774971061</v>
       </c>
       <c r="F66">
-        <v>0.3661925211209399</v>
+        <v>0.36619252112093992</v>
       </c>
       <c r="G66">
-        <v>-0.2646244635515607</v>
+        <v>-0.26462446355156072</v>
       </c>
       <c r="H66" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -2719,16 +2742,16 @@
         <v>258.0086206079614</v>
       </c>
       <c r="F67">
-        <v>0.3787916372177544</v>
+        <v>0.37879163721775438</v>
       </c>
       <c r="G67">
-        <v>-0.2520253474547461</v>
+        <v>-0.25202534745474608</v>
       </c>
       <c r="H67" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -2739,22 +2762,22 @@
         <v>146</v>
       </c>
       <c r="D68">
-        <v>30.877</v>
+        <v>30.876999999999999</v>
       </c>
       <c r="E68">
-        <v>235.6799559542702</v>
+        <v>235.67995595427021</v>
       </c>
       <c r="F68">
-        <v>0.336589482939546</v>
+        <v>0.33658948293954599</v>
       </c>
       <c r="G68">
-        <v>-0.2942275017329546</v>
+        <v>-0.29422750173295459</v>
       </c>
       <c r="H68" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -2765,22 +2788,22 @@
         <v>147</v>
       </c>
       <c r="D69">
-        <v>75180.40900000001</v>
+        <v>75180.409000000014</v>
       </c>
       <c r="E69">
-        <v>244.8335976730318</v>
+        <v>244.83359767303179</v>
       </c>
       <c r="F69">
-        <v>0.5369310916167438</v>
+        <v>0.53693109161674379</v>
       </c>
       <c r="G69">
-        <v>-0.09388589305575679</v>
+        <v>-9.3885893055756786E-2</v>
       </c>
       <c r="H69" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -2791,22 +2814,22 @@
         <v>148</v>
       </c>
       <c r="D70">
-        <v>2763.484999999999</v>
+        <v>2763.4849999999992</v>
       </c>
       <c r="E70">
         <v>324.7422946026486</v>
       </c>
       <c r="F70">
-        <v>0.2974794893240567</v>
+        <v>0.29747948932405671</v>
       </c>
       <c r="G70">
-        <v>-0.3333374953484439</v>
+        <v>-0.33333749534844392</v>
       </c>
       <c r="H70" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -2823,16 +2846,16 @@
         <v>1011.186490436721</v>
       </c>
       <c r="F71">
-        <v>0.2491985997761378</v>
+        <v>0.24919859977613781</v>
       </c>
       <c r="G71">
-        <v>-0.3816183848963627</v>
+        <v>-0.38161838489636268</v>
       </c>
       <c r="H71" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -2843,22 +2866,22 @@
         <v>150</v>
       </c>
       <c r="D72">
-        <v>519.7999999999998</v>
+        <v>519.79999999999984</v>
       </c>
       <c r="E72">
-        <v>263.2285109657561</v>
+        <v>263.22851096575607</v>
       </c>
       <c r="F72">
-        <v>0.2235231922360905</v>
+        <v>0.22352319223609049</v>
       </c>
       <c r="G72">
-        <v>-0.4072937924364101</v>
+        <v>-0.40729379243641012</v>
       </c>
       <c r="H72" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -2872,19 +2895,19 @@
         <v>1220.451</v>
       </c>
       <c r="E73">
-        <v>347.6299007498048</v>
+        <v>347.62990074980479</v>
       </c>
       <c r="F73">
-        <v>0.390893175643698</v>
+        <v>0.39089317564369802</v>
       </c>
       <c r="G73">
-        <v>-0.2399238090288026</v>
+        <v>-0.23992380902880259</v>
       </c>
       <c r="H73" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -2901,16 +2924,16 @@
         <v>236.7002239340959</v>
       </c>
       <c r="F74">
-        <v>0.3329908570871202</v>
+        <v>0.33299085708712017</v>
       </c>
       <c r="G74">
-        <v>-0.2978261275853804</v>
+        <v>-0.29782612758538041</v>
       </c>
       <c r="H74" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -2921,22 +2944,22 @@
         <v>153</v>
       </c>
       <c r="D75">
-        <v>60.03999999999999</v>
+        <v>60.039999999999992</v>
       </c>
       <c r="E75">
-        <v>204.0434710193205</v>
+        <v>204.04347101932049</v>
       </c>
       <c r="F75">
-        <v>0.2906250254873989</v>
+        <v>0.29062502548739888</v>
       </c>
       <c r="G75">
-        <v>-0.3401919591851016</v>
+        <v>-0.34019195918510159</v>
       </c>
       <c r="H75" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -2947,13 +2970,13 @@
         <v>154</v>
       </c>
       <c r="D76">
-        <v>14101.56299999997</v>
+        <v>14101.562999999969</v>
       </c>
       <c r="E76">
         <v>227.680616680577</v>
       </c>
       <c r="F76">
-        <v>0.3184834263740979</v>
+        <v>0.31848342637409788</v>
       </c>
       <c r="G76">
         <v>-0.3123335582984027</v>
@@ -2962,7 +2985,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -2973,13 +2996,13 @@
         <v>155</v>
       </c>
       <c r="D77">
-        <v>2585.468999999999</v>
+        <v>2585.4689999999991</v>
       </c>
       <c r="E77">
-        <v>302.7852432189288</v>
+        <v>302.78524321892883</v>
       </c>
       <c r="F77">
-        <v>0.4131793204027862</v>
+        <v>0.41317932040278621</v>
       </c>
       <c r="G77">
         <v>-0.2176376642697144</v>
@@ -2988,7 +3011,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -3002,19 +3025,19 @@
         <v>856.8490000000005</v>
       </c>
       <c r="E78">
-        <v>217.0080492595544</v>
+        <v>217.00804925955441</v>
       </c>
       <c r="F78">
-        <v>0.3513099965186861</v>
+        <v>0.35130999651868611</v>
       </c>
       <c r="G78">
-        <v>-0.2795069881538145</v>
+        <v>-0.27950698815381447</v>
       </c>
       <c r="H78" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -3025,22 +3048,22 @@
         <v>157</v>
       </c>
       <c r="D79">
-        <v>945.2780000000001</v>
+        <v>945.27800000000013</v>
       </c>
       <c r="E79">
         <v>225.0900370049869</v>
       </c>
       <c r="F79">
-        <v>0.3250482135347725</v>
+        <v>0.32504821353477248</v>
       </c>
       <c r="G79">
-        <v>-0.305768771137728</v>
+        <v>-0.30576877113772799</v>
       </c>
       <c r="H79" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -3051,22 +3074,22 @@
         <v>158</v>
       </c>
       <c r="D80">
-        <v>382.4149999999998</v>
+        <v>382.41499999999979</v>
       </c>
       <c r="E80">
-        <v>244.9198122458586</v>
+        <v>244.91981224585859</v>
       </c>
       <c r="F80">
-        <v>0.3452803921496422</v>
+        <v>0.34528039214964218</v>
       </c>
       <c r="G80">
-        <v>-0.2855365925228583</v>
+        <v>-0.28553659252285829</v>
       </c>
       <c r="H80" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -3080,19 +3103,19 @@
         <v>72527.92999999992</v>
       </c>
       <c r="E81">
-        <v>220.9026914183277</v>
+        <v>220.90269141832769</v>
       </c>
       <c r="F81">
-        <v>0.3102025650284839</v>
+        <v>0.31020256502848392</v>
       </c>
       <c r="G81">
-        <v>-0.3206144196440167</v>
+        <v>-0.32061441964401671</v>
       </c>
       <c r="H81" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -3103,13 +3126,13 @@
         <v>160</v>
       </c>
       <c r="D82">
-        <v>31.301</v>
+        <v>31.300999999999998</v>
       </c>
       <c r="E82">
-        <v>507.1777259512475</v>
+        <v>507.17772595124751</v>
       </c>
       <c r="F82">
-        <v>0.3042684194572647</v>
+        <v>0.30426841945726468</v>
       </c>
       <c r="G82">
         <v>-0.3265485652152359</v>
@@ -3118,7 +3141,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -3132,19 +3155,19 @@
         <v>134.453</v>
       </c>
       <c r="E83">
-        <v>240.6884190014354</v>
+        <v>240.68841900143539</v>
       </c>
       <c r="F83">
-        <v>0.2987179691182933</v>
+        <v>0.29871796911829329</v>
       </c>
       <c r="G83">
-        <v>-0.3320990155542073</v>
+        <v>-0.33209901555420729</v>
       </c>
       <c r="H83" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -3155,22 +3178,22 @@
         <v>162</v>
       </c>
       <c r="D84">
-        <v>549.7500000000001</v>
+        <v>549.75000000000011</v>
       </c>
       <c r="E84">
-        <v>195.3111232378353</v>
+        <v>195.31112323783529</v>
       </c>
       <c r="F84">
-        <v>0.2624243013338609</v>
+        <v>0.26242430133386091</v>
       </c>
       <c r="G84">
-        <v>-0.3683926833386397</v>
+        <v>-0.36839268333863973</v>
       </c>
       <c r="H84" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -3184,19 +3207,19 @@
         <v>1652.645</v>
       </c>
       <c r="E85">
-        <v>300.8146153590153</v>
+        <v>300.81461535901531</v>
       </c>
       <c r="F85">
-        <v>0.3941925151078149</v>
+        <v>0.39419251510781489</v>
       </c>
       <c r="G85">
-        <v>-0.2366244695646856</v>
+        <v>-0.23662446956468561</v>
       </c>
       <c r="H85" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -3207,22 +3230,22 @@
         <v>164</v>
       </c>
       <c r="D86">
-        <v>7032.772999999997</v>
+        <v>7032.7729999999974</v>
       </c>
       <c r="E86">
-        <v>192.7193683060725</v>
+        <v>192.71936830607251</v>
       </c>
       <c r="F86">
-        <v>0.2493422506680253</v>
+        <v>0.24934225066802529</v>
       </c>
       <c r="G86">
-        <v>-0.3814747340044753</v>
+        <v>-0.38147473400447529</v>
       </c>
       <c r="H86" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -3239,7 +3262,7 @@
         <v>192.3460877042132</v>
       </c>
       <c r="F87">
-        <v>0.1613518495687102</v>
+        <v>0.16135184956871021</v>
       </c>
       <c r="G87">
         <v>-0.4694651351037904</v>
@@ -3248,7 +3271,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -3259,22 +3282,22 @@
         <v>166</v>
       </c>
       <c r="D88">
-        <v>299.753</v>
+        <v>299.75299999999999</v>
       </c>
       <c r="E88">
-        <v>598.0469586626322</v>
+        <v>598.04695866263216</v>
       </c>
       <c r="F88">
-        <v>0.3301653339612048</v>
+        <v>0.33016533396120479</v>
       </c>
       <c r="G88">
-        <v>-0.3006516507112957</v>
+        <v>-0.30065165071129568</v>
       </c>
       <c r="H88" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -3285,22 +3308,22 @@
         <v>167</v>
       </c>
       <c r="D89">
-        <v>335.2769999999999</v>
+        <v>335.27699999999987</v>
       </c>
       <c r="E89">
-        <v>297.159960271656</v>
+        <v>297.15996027165602</v>
       </c>
       <c r="F89">
-        <v>0.1645936228944775</v>
+        <v>0.16459362289447749</v>
       </c>
       <c r="G89">
-        <v>-0.466223361778023</v>
+        <v>-0.46622336177802298</v>
       </c>
       <c r="H89" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -3311,22 +3334,22 @@
         <v>168</v>
       </c>
       <c r="D90">
-        <v>83.221</v>
+        <v>83.221000000000004</v>
       </c>
       <c r="E90">
-        <v>723.2113288713185</v>
+        <v>723.21132887131853</v>
       </c>
       <c r="F90">
-        <v>0.4421915339692908</v>
+        <v>0.44219153396929078</v>
       </c>
       <c r="G90">
-        <v>-0.1886254507032097</v>
+        <v>-0.18862545070320971</v>
       </c>
       <c r="H90" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -3340,19 +3363,19 @@
         <v>5570.747000000003</v>
       </c>
       <c r="E91">
-        <v>260.4009103267479</v>
+        <v>260.40091032674792</v>
       </c>
       <c r="F91">
-        <v>0.4444027639003358</v>
+        <v>0.44440276390033578</v>
       </c>
       <c r="G91">
-        <v>-0.1864142207721647</v>
+        <v>-0.18641422077216471</v>
       </c>
       <c r="H91" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -3363,22 +3386,22 @@
         <v>170</v>
       </c>
       <c r="D92">
-        <v>638.1449999999999</v>
+        <v>638.14499999999987</v>
       </c>
       <c r="E92">
-        <v>225.8238488117904</v>
+        <v>225.82384881179041</v>
       </c>
       <c r="F92">
-        <v>0.4481218747133359</v>
+        <v>0.44812187471333592</v>
       </c>
       <c r="G92">
-        <v>-0.1826951099591647</v>
+        <v>-0.18269510995916469</v>
       </c>
       <c r="H92" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -3389,22 +3412,22 @@
         <v>171</v>
       </c>
       <c r="D93">
-        <v>28788.96699999998</v>
+        <v>28788.966999999979</v>
       </c>
       <c r="E93">
-        <v>247.8202073037214</v>
+        <v>247.82020730372139</v>
       </c>
       <c r="F93">
-        <v>0.4902767865624683</v>
+        <v>0.49027678656246831</v>
       </c>
       <c r="G93">
-        <v>-0.1405401981100323</v>
+        <v>-0.14054019811003229</v>
       </c>
       <c r="H93" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -3415,22 +3438,22 @@
         <v>172</v>
       </c>
       <c r="D94">
-        <v>3626.865999999996</v>
+        <v>3626.8659999999959</v>
       </c>
       <c r="E94">
-        <v>347.7238502883762</v>
+        <v>347.72385028837618</v>
       </c>
       <c r="F94">
-        <v>0.2476909057217691</v>
+        <v>0.24769090572176911</v>
       </c>
       <c r="G94">
-        <v>-0.3831260789507315</v>
+        <v>-0.38312607895073147</v>
       </c>
       <c r="H94" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -3441,22 +3464,22 @@
         <v>173</v>
       </c>
       <c r="D95">
-        <v>10565.02599999999</v>
+        <v>10565.025999999991</v>
       </c>
       <c r="E95">
-        <v>366.0767649790928</v>
+        <v>366.07676497909279</v>
       </c>
       <c r="F95">
-        <v>0.2633570005029258</v>
+        <v>0.26335700050292582</v>
       </c>
       <c r="G95">
-        <v>-0.3674599841695748</v>
+        <v>-0.36745998416957482</v>
       </c>
       <c r="H95" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -3467,22 +3490,22 @@
         <v>174</v>
       </c>
       <c r="D96">
-        <v>89.24599999999998</v>
+        <v>89.245999999999981</v>
       </c>
       <c r="E96">
-        <v>239.778141317258</v>
+        <v>239.77814131725799</v>
       </c>
       <c r="F96">
-        <v>0.3079558770186666</v>
+        <v>0.30795587701866661</v>
       </c>
       <c r="G96">
-        <v>-0.322861107653834</v>
+        <v>-0.32286110765383402</v>
       </c>
       <c r="H96" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>8</v>
       </c>
@@ -3493,22 +3516,22 @@
         <v>175</v>
       </c>
       <c r="D97">
-        <v>57896.57899999996</v>
+        <v>57896.578999999962</v>
       </c>
       <c r="E97">
-        <v>179.9980684523695</v>
+        <v>179.99806845236949</v>
       </c>
       <c r="F97">
         <v>1.02752699258098</v>
       </c>
       <c r="G97">
-        <v>0.3967100079084792</v>
+        <v>0.39671000790847921</v>
       </c>
       <c r="H97" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>8</v>
       </c>
@@ -3522,19 +3545,19 @@
         <v>11996.501</v>
       </c>
       <c r="E98">
-        <v>257.1624067717747</v>
+        <v>257.16240677177473</v>
       </c>
       <c r="F98">
-        <v>0.3309351271967285</v>
+        <v>0.33093512719672852</v>
       </c>
       <c r="G98">
-        <v>-0.2998818574757721</v>
+        <v>-0.29988185747577212</v>
       </c>
       <c r="H98" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -3545,13 +3568,13 @@
         <v>177</v>
       </c>
       <c r="D99">
-        <v>642.591</v>
+        <v>642.59100000000001</v>
       </c>
       <c r="E99">
-        <v>440.1672136709043</v>
+        <v>440.16721367090429</v>
       </c>
       <c r="F99">
-        <v>0.3639273460848891</v>
+        <v>0.36392734608488908</v>
       </c>
       <c r="G99">
         <v>-0.2668896385876115</v>
@@ -3560,7 +3583,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>8</v>
       </c>
@@ -3571,22 +3594,22 @@
         <v>178</v>
       </c>
       <c r="D100">
-        <v>20.015</v>
+        <v>20.015000000000001</v>
       </c>
       <c r="E100">
-        <v>297.7262053459905</v>
+        <v>297.72620534599048</v>
       </c>
       <c r="F100">
-        <v>0.2482443948531055</v>
+        <v>0.24824439485310551</v>
       </c>
       <c r="G100">
-        <v>-0.382572589819395</v>
+        <v>-0.38257258981939501</v>
       </c>
       <c r="H100" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>8</v>
       </c>
@@ -3597,13 +3620,13 @@
         <v>179</v>
       </c>
       <c r="D101">
-        <v>6.171</v>
+        <v>6.1710000000000003</v>
       </c>
       <c r="E101">
         <v>109.5802949278885</v>
       </c>
       <c r="F101">
-        <v>0.1534336174249721</v>
+        <v>0.15343361742497211</v>
       </c>
       <c r="G101">
         <v>-0.4773833672475285</v>
@@ -3612,7 +3635,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>8</v>
       </c>
@@ -3626,19 +3649,19 @@
         <v>25387.68400000007</v>
       </c>
       <c r="E102">
-        <v>251.933466636814</v>
+        <v>251.93346663681399</v>
       </c>
       <c r="F102">
-        <v>0.4043797978799994</v>
+        <v>0.40437979787999939</v>
       </c>
       <c r="G102">
-        <v>-0.2264371867925012</v>
+        <v>-0.22643718679250119</v>
       </c>
       <c r="H102" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>8</v>
       </c>
@@ -3649,13 +3672,13 @@
         <v>181</v>
       </c>
       <c r="D103">
-        <v>5826.660000000006</v>
+        <v>5826.6600000000062</v>
       </c>
       <c r="E103">
-        <v>309.4800125629432</v>
+        <v>309.48001256294322</v>
       </c>
       <c r="F103">
-        <v>0.4994029571775767</v>
+        <v>0.49940295717757671</v>
       </c>
       <c r="G103">
         <v>-0.1314140274949239</v>
@@ -3664,7 +3687,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>8</v>
       </c>
@@ -3678,19 +3701,19 @@
         <v>16033.087</v>
       </c>
       <c r="E104">
-        <v>308.1500468375176</v>
+        <v>308.15004683751761</v>
       </c>
       <c r="F104">
-        <v>0.4914234882331401</v>
+        <v>0.49142348823314008</v>
       </c>
       <c r="G104">
-        <v>-0.1393934964393604</v>
+        <v>-0.13939349643936039</v>
       </c>
       <c r="H104" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>8</v>
       </c>
@@ -3701,22 +3724,22 @@
         <v>183</v>
       </c>
       <c r="D105">
-        <v>2179.456</v>
+        <v>2179.4560000000001</v>
       </c>
       <c r="E105">
-        <v>220.1772093586658</v>
+        <v>220.17720935866581</v>
       </c>
       <c r="F105">
-        <v>0.3628072677037888</v>
+        <v>0.36280726770378879</v>
       </c>
       <c r="G105">
-        <v>-0.2680097169687117</v>
+        <v>-0.26800971696871168</v>
       </c>
       <c r="H105" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>8</v>
       </c>
@@ -3727,22 +3750,22 @@
         <v>184</v>
       </c>
       <c r="D106">
-        <v>2.162</v>
+        <v>2.1619999999999999</v>
       </c>
       <c r="E106">
         <v>104.7178538390379</v>
       </c>
       <c r="F106">
-        <v>0.1468652405809626</v>
+        <v>0.14686524058096259</v>
       </c>
       <c r="G106">
-        <v>-0.483951744091538</v>
+        <v>-0.48395174409153802</v>
       </c>
       <c r="H106" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>8</v>
       </c>
@@ -3753,13 +3776,13 @@
         <v>185</v>
       </c>
       <c r="D107">
-        <v>2100.931999999999</v>
+        <v>2100.9319999999989</v>
       </c>
       <c r="E107">
-        <v>225.8961213404339</v>
+        <v>225.89612134043389</v>
       </c>
       <c r="F107">
-        <v>0.3164360776107273</v>
+        <v>0.31643607761072728</v>
       </c>
       <c r="G107">
         <v>-0.3143809070617733</v>
@@ -3768,7 +3791,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>8</v>
       </c>
@@ -3779,22 +3802,22 @@
         <v>186</v>
       </c>
       <c r="D108">
-        <v>654.5389999999998</v>
+        <v>654.53899999999976</v>
       </c>
       <c r="E108">
-        <v>193.8324072362381</v>
+        <v>193.83240723623811</v>
       </c>
       <c r="F108">
         <v>0.2684068290172083</v>
       </c>
       <c r="G108">
-        <v>-0.3624101556552923</v>
+        <v>-0.36241015565529228</v>
       </c>
       <c r="H108" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>8</v>
       </c>
@@ -3808,19 +3831,19 @@
         <v>36.28</v>
       </c>
       <c r="E109">
-        <v>201.4098676957001</v>
+        <v>201.40986769570009</v>
       </c>
       <c r="F109">
-        <v>0.2830356513234853</v>
+        <v>0.28303565132348529</v>
       </c>
       <c r="G109">
-        <v>-0.3477813333490152</v>
+        <v>-0.34778133334901518</v>
       </c>
       <c r="H109" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -3831,22 +3854,22 @@
         <v>188</v>
       </c>
       <c r="D110">
-        <v>6665.726000000011</v>
+        <v>6665.7260000000106</v>
       </c>
       <c r="E110">
         <v>254.168608190615</v>
       </c>
       <c r="F110">
-        <v>0.3578519028057514</v>
+        <v>0.35785190280575141</v>
       </c>
       <c r="G110">
-        <v>-0.2729650818667492</v>
+        <v>-0.27296508186674923</v>
       </c>
       <c r="H110" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>8</v>
       </c>
@@ -3863,16 +3886,16 @@
         <v>252.0403023310009</v>
       </c>
       <c r="F111">
-        <v>0.3622976091189594</v>
+        <v>0.36229760911895942</v>
       </c>
       <c r="G111">
-        <v>-0.2685193755535412</v>
+        <v>-0.26851937555354122</v>
       </c>
       <c r="H111" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -3883,22 +3906,22 @@
         <v>190</v>
       </c>
       <c r="D112">
-        <v>1363.005999999999</v>
+        <v>1363.0059999999989</v>
       </c>
       <c r="E112">
-        <v>344.1076341556825</v>
+        <v>344.10763415568249</v>
       </c>
       <c r="F112">
         <v>0.2587030357693057</v>
       </c>
       <c r="G112">
-        <v>-0.3721139489031949</v>
+        <v>-0.37211394890319488</v>
       </c>
       <c r="H112" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>8</v>
       </c>
@@ -3909,22 +3932,22 @@
         <v>191</v>
       </c>
       <c r="D113">
-        <v>21754.99599999999</v>
+        <v>21754.995999999988</v>
       </c>
       <c r="E113">
-        <v>286.52056796517</v>
+        <v>286.52056796517002</v>
       </c>
       <c r="F113">
-        <v>0.2612493917977798</v>
+        <v>0.26124939179777978</v>
       </c>
       <c r="G113">
-        <v>-0.3695675928747207</v>
+        <v>-0.36956759287472069</v>
       </c>
       <c r="H113" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -3935,22 +3958,22 @@
         <v>192</v>
       </c>
       <c r="D114">
-        <v>31.691</v>
+        <v>31.690999999999999</v>
       </c>
       <c r="E114">
-        <v>466.1698905051907</v>
+        <v>466.16989050519072</v>
       </c>
       <c r="F114">
         <v>0.3477117867179173</v>
       </c>
       <c r="G114">
-        <v>-0.2831051979545833</v>
+        <v>-0.28310519795458328</v>
       </c>
       <c r="H114" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>8</v>
       </c>
@@ -3961,22 +3984,22 @@
         <v>193</v>
       </c>
       <c r="D115">
-        <v>64465.26800000089</v>
+        <v>64465.268000000891</v>
       </c>
       <c r="E115">
-        <v>246.9107763578967</v>
+        <v>246.91077635789671</v>
       </c>
       <c r="F115">
-        <v>0.4774137953956469</v>
+        <v>0.47741379539564688</v>
       </c>
       <c r="G115">
-        <v>-0.1534031892768536</v>
+        <v>-0.15340318927685359</v>
       </c>
       <c r="H115" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -3987,22 +4010,22 @@
         <v>194</v>
       </c>
       <c r="D116">
-        <v>24405.47699999999</v>
+        <v>24405.476999999992</v>
       </c>
       <c r="E116">
-        <v>263.3829611279472</v>
+        <v>263.38296112794723</v>
       </c>
       <c r="F116">
-        <v>0.4950854070582414</v>
+        <v>0.49508540705824139</v>
       </c>
       <c r="G116">
-        <v>-0.1357315776142591</v>
+        <v>-0.13573157761425911</v>
       </c>
       <c r="H116" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>8</v>
       </c>
@@ -4016,19 +4039,19 @@
         <v>1646.530999999999</v>
       </c>
       <c r="E117">
-        <v>228.1344839544475</v>
+        <v>228.13448395444749</v>
       </c>
       <c r="F117">
-        <v>0.4379344060645952</v>
+        <v>0.43793440606459522</v>
       </c>
       <c r="G117">
-        <v>-0.1928825786079054</v>
+        <v>-0.19288257860790539</v>
       </c>
       <c r="H117" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>8</v>
       </c>
@@ -4042,19 +4065,19 @@
         <v>2114.694</v>
       </c>
       <c r="E118">
-        <v>676.979572458237</v>
+        <v>676.97957245823704</v>
       </c>
       <c r="F118">
-        <v>0.2820238225496872</v>
+        <v>0.28202382254968722</v>
       </c>
       <c r="G118">
-        <v>-0.3487931621228134</v>
+        <v>-0.34879316212281342</v>
       </c>
       <c r="H118" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -4065,22 +4088,22 @@
         <v>197</v>
       </c>
       <c r="D119">
-        <v>8282.056000000011</v>
+        <v>8282.0560000000114</v>
       </c>
       <c r="E119">
-        <v>151.3531893529818</v>
+        <v>151.35318935298179</v>
       </c>
       <c r="F119">
-        <v>0.3674182929743637</v>
+        <v>0.36741829297436368</v>
       </c>
       <c r="G119">
-        <v>-0.2633986916981368</v>
+        <v>-0.26339869169813679</v>
       </c>
       <c r="H119" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>8</v>
       </c>
@@ -4091,22 +4114,22 @@
         <v>198</v>
       </c>
       <c r="D120">
-        <v>582.5799999999999</v>
+        <v>582.57999999999993</v>
       </c>
       <c r="E120">
-        <v>184.8000102990148</v>
+        <v>184.80001029901479</v>
       </c>
       <c r="F120">
-        <v>0.4196566679512553</v>
+        <v>0.41965666795125528</v>
       </c>
       <c r="G120">
-        <v>-0.2111603167212452</v>
+        <v>-0.21116031672124519</v>
       </c>
       <c r="H120" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>8</v>
       </c>
@@ -4117,13 +4140,13 @@
         <v>199</v>
       </c>
       <c r="D121">
-        <v>22595.85100000003</v>
+        <v>22595.851000000031</v>
       </c>
       <c r="E121">
-        <v>189.8202466461649</v>
+        <v>189.82024664616489</v>
       </c>
       <c r="F121">
-        <v>0.4577069990503776</v>
+        <v>0.45770699905037759</v>
       </c>
       <c r="G121">
         <v>-0.1731099856221229</v>
@@ -4132,7 +4155,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>9</v>
       </c>

</xml_diff>